<commit_message>
Cambios en el Readme
</commit_message>
<xml_diff>
--- a/prov.xlsx
+++ b/prov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\practicas\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\practicas\practicas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>http://www.rodamientos-samper.com.mx/</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Ave.Adolfo B. Horn Jr No. 3506 Col. Toluquilla C.P. 45640 Tlajomulco de Zúñiga, Jal.</t>
+  </si>
+  <si>
+    <t>Material 1</t>
   </si>
 </sst>
 </file>
@@ -324,6 +327,7 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -337,7 +341,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -363,16 +366,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:H17" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:H17" totalsRowShown="0" dataDxfId="7">
   <autoFilter ref="B3:H17"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Proveedores" dataDxfId="7"/>
-    <tableColumn id="2" name="Columna1" dataDxfId="6"/>
-    <tableColumn id="3" name="Columna2" dataDxfId="5"/>
-    <tableColumn id="4" name="Columna3" dataDxfId="4"/>
-    <tableColumn id="5" name="Columna4" dataDxfId="3"/>
-    <tableColumn id="6" name="Direccion " dataDxfId="2"/>
-    <tableColumn id="7" name="Columna6" dataDxfId="1"/>
+    <tableColumn id="1" name="Proveedores" dataDxfId="6"/>
+    <tableColumn id="2" name="Columna1" dataDxfId="5"/>
+    <tableColumn id="3" name="Columna2" dataDxfId="4"/>
+    <tableColumn id="4" name="Columna3" dataDxfId="3"/>
+    <tableColumn id="5" name="Columna4" dataDxfId="2"/>
+    <tableColumn id="6" name="Direccion " dataDxfId="1"/>
+    <tableColumn id="7" name="Columna6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -658,7 +661,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H21"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
@@ -907,6 +910,11 @@
         <v>34</v>
       </c>
     </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Readme y excel Modificado
</commit_message>
<xml_diff>
--- a/prov.xlsx
+++ b/prov.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>http://www.rodamientos-samper.com.mx/</t>
   </si>
@@ -32,18 +32,6 @@
     <t>Columna1</t>
   </si>
   <si>
-    <t>Columna2</t>
-  </si>
-  <si>
-    <t>Columna3</t>
-  </si>
-  <si>
-    <t>Columna4</t>
-  </si>
-  <si>
-    <t>Columna6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rodamientos SAMPER </t>
   </si>
   <si>
@@ -153,6 +141,54 @@
   </si>
   <si>
     <t>Material 1</t>
+  </si>
+  <si>
+    <t>Grupo Palme</t>
+  </si>
+  <si>
+    <t>http://www.palme.mx/</t>
+  </si>
+  <si>
+    <t>Calle 1 Norte lote 2 M bis Colonia Fondeport C.P. 28219 Manzanillo , Colima</t>
+  </si>
+  <si>
+    <t>(314) 336-526</t>
+  </si>
+  <si>
+    <t>ventasman@palme.com.mx</t>
+  </si>
+  <si>
+    <t>Grupo Infra</t>
+  </si>
+  <si>
+    <t>http://grupoinfra.com/</t>
+  </si>
+  <si>
+    <t>Calle 1 Lote 2-B Manzana 1 Col. Parque Industrial Fondeport Manzanillo COL 28219</t>
+  </si>
+  <si>
+    <t>(314) 336 53 84, (314) 336 53 89</t>
+  </si>
+  <si>
+    <t>Ferrepacifico</t>
+  </si>
+  <si>
+    <t>http://sitio.ferrepacifico.com.mx</t>
+  </si>
+  <si>
+    <t>Dirección: Blvd. Miguel de la Madrid H. #472 Frente al Parque Fondeport</t>
+  </si>
+  <si>
+    <t>(314) 33 12131 al 40 [Con 10 Líneas]</t>
+  </si>
+  <si>
+    <t>Pagina web</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Correo</t>
   </si>
 </sst>
 </file>
@@ -213,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -241,25 +277,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <strike val="0"/>
@@ -366,16 +398,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:H17" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="B3:H17"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Proveedores" dataDxfId="6"/>
-    <tableColumn id="2" name="Columna1" dataDxfId="5"/>
-    <tableColumn id="3" name="Columna2" dataDxfId="4"/>
-    <tableColumn id="4" name="Columna3" dataDxfId="3"/>
-    <tableColumn id="5" name="Columna4" dataDxfId="2"/>
-    <tableColumn id="6" name="Direccion " dataDxfId="1"/>
-    <tableColumn id="7" name="Columna6" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B3:G18" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="B3:G18"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Proveedores" dataDxfId="5"/>
+    <tableColumn id="2" name="Columna1" dataDxfId="4"/>
+    <tableColumn id="3" name="Pagina web" dataDxfId="3"/>
+    <tableColumn id="4" name="Telefono" dataDxfId="2"/>
+    <tableColumn id="5" name="Correo" dataDxfId="1"/>
+    <tableColumn id="6" name="Direccion " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -663,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,174 +711,197 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="57" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="2:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="2:8" ht="57" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="2:8" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="2:8" ht="71.25" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="2:8" ht="57" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
+    <row r="11" spans="2:8" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+    <row r="12" spans="2:8" ht="57" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -855,8 +909,8 @@
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -864,8 +918,8 @@
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -873,8 +927,8 @@
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -888,31 +942,39 @@
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
     </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
         <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>